<commit_message>
feat: Add get_URLs function for extracting embedded links from Excel
</commit_message>
<xml_diff>
--- a/chargemasters/chargemaster_index.xlsx
+++ b/chargemasters/chargemaster_index.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emigre459/Documents/gitProjects/Hospital Pricing Data/chargemasters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F5C778-C230-5B49-ACFE-EC6CD31A75B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6ECBD77-7DFD-CD45-9E30-430D4C5EAAB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" xr2:uid="{92AE58A8-9246-5F4D-A35E-9423D4435357}"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="25600" windowHeight="14580" xr2:uid="{92AE58A8-9246-5F4D-A35E-9423D4435357}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4214,7 +4214,18 @@
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -4527,8 +4538,8 @@
   <dimension ref="A1:F2067"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B839" sqref="B839"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25072,6 +25083,9 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C34" r:id="rId1" xr:uid="{674DF260-F5ED-8742-ACB5-BB5D903AF1C9}"/>
     <hyperlink ref="C54" r:id="rId2" xr:uid="{D6A604CF-8AB4-2E48-8630-D623484D9646}"/>

</xml_diff>